<commit_message>
Se actualizó el proyecto grupal siguiendo las nuevas instrucciones
</commit_message>
<xml_diff>
--- a/Proyecto Grupal/Datos.xlsx
+++ b/Proyecto Grupal/Datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erick-sc\Desktop\IQ0333 1000\I-2021\Trabajo Grupal\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\Repositories\an-lisis_procesos_ii\Proyecto Grupal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1164891-1169-4253-A58F-E7074BBFF949}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC0E738-1CDC-47EE-848A-7A8151B7A78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21285" yWindow="-4590" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos finales" sheetId="5" r:id="rId1"/>
@@ -472,30 +472,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CE6CDE5-BF92-4D29-9775-8E7F742ADF07}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L26"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5:K26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.90625" style="2"/>
-    <col min="3" max="4" width="14.26953125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.90625" style="2"/>
-    <col min="6" max="7" width="15.1796875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.90625" style="2"/>
-    <col min="9" max="10" width="15.08984375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="10.90625" style="2"/>
-    <col min="12" max="12" width="14.26953125" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="10.90625" style="2"/>
+    <col min="2" max="2" width="10.85546875" style="2"/>
+    <col min="3" max="4" width="14.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="2"/>
+    <col min="6" max="7" width="15.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="2"/>
+    <col min="9" max="10" width="15.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" style="2"/>
+    <col min="12" max="12" width="14.28515625" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -517,7 +517,7 @@
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -555,7 +555,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -593,7 +593,7 @@
         <v>30.8</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -631,7 +631,7 @@
         <v>47.4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>10</v>
       </c>
@@ -669,7 +669,7 @@
         <v>52.3</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>15</v>
       </c>
@@ -707,7 +707,7 @@
         <v>58.3</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>20</v>
       </c>
@@ -745,7 +745,7 @@
         <v>61.8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>25</v>
       </c>
@@ -783,7 +783,7 @@
         <v>67.099999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>30</v>
       </c>
@@ -821,7 +821,7 @@
         <v>72.900000000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>35</v>
       </c>
@@ -859,7 +859,7 @@
         <v>80.599999999999994</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>40</v>
       </c>
@@ -897,7 +897,7 @@
         <v>90.5</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>45</v>
       </c>
@@ -935,7 +935,7 @@
         <v>95.8</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>50</v>
       </c>
@@ -973,7 +973,7 @@
         <v>103.7</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>55</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>110.5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>60</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>114.5</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>65</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>123.8</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>70</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>130.69999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>75</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>80</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>146.5</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>85</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>155.6</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>90</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>91.2</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>95</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>191.2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>99.9</v>
       </c>

</xml_diff>

<commit_message>
Se implementó ANOVA por medio de Python para poder extraer los resultados que se requieren para terminar el proyecto
</commit_message>
<xml_diff>
--- a/Proyecto Grupal/Datos.xlsx
+++ b/Proyecto Grupal/Datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\Repositories\an-lisis_procesos_ii\Proyecto Grupal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC0E738-1CDC-47EE-848A-7A8151B7A78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2626DCCF-D2C9-4FAB-9E06-A65C804DDC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21285" yWindow="-4590" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos finales" sheetId="5" r:id="rId1"/>
@@ -113,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -132,6 +132,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CE6CDE5-BF92-4D29-9775-8E7F742ADF07}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:K26"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5:M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,12 +491,12 @@
     <col min="13" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -517,7 +518,7 @@
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:12" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -555,7 +556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -592,8 +593,12 @@
       <c r="L5" s="1">
         <v>30.8</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="8">
+        <f>AVERAGE(K5,E5,B5)</f>
+        <v>375.33333333333331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -630,8 +635,12 @@
       <c r="L6" s="1">
         <v>47.4</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="8">
+        <f t="shared" ref="M6:M26" si="0">AVERAGE(K6,E6,B6)</f>
+        <v>461</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>10</v>
       </c>
@@ -668,8 +677,12 @@
       <c r="L7" s="1">
         <v>52.3</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="8">
+        <f t="shared" si="0"/>
+        <v>531.83333333333337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>15</v>
       </c>
@@ -706,8 +719,12 @@
       <c r="L8" s="1">
         <v>58.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="8">
+        <f t="shared" si="0"/>
+        <v>602.13333333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>20</v>
       </c>
@@ -744,8 +761,12 @@
       <c r="L9" s="1">
         <v>61.8</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="8">
+        <f t="shared" si="0"/>
+        <v>676.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>25</v>
       </c>
@@ -782,8 +803,12 @@
       <c r="L10" s="1">
         <v>67.099999999999994</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="8">
+        <f t="shared" si="0"/>
+        <v>751.06666666666661</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>30</v>
       </c>
@@ -820,8 +845,12 @@
       <c r="L11" s="1">
         <v>72.900000000000006</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="8">
+        <f t="shared" si="0"/>
+        <v>822.4666666666667</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>35</v>
       </c>
@@ -858,8 +887,12 @@
       <c r="L12" s="1">
         <v>80.599999999999994</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" s="8">
+        <f t="shared" si="0"/>
+        <v>893.86666666666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>40</v>
       </c>
@@ -896,8 +929,12 @@
       <c r="L13" s="1">
         <v>90.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" s="8">
+        <f t="shared" si="0"/>
+        <v>967.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>45</v>
       </c>
@@ -934,8 +971,12 @@
       <c r="L14" s="1">
         <v>95.8</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" s="8">
+        <f t="shared" si="0"/>
+        <v>1040.3000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>50</v>
       </c>
@@ -972,8 +1013,12 @@
       <c r="L15" s="1">
         <v>103.7</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" s="8">
+        <f t="shared" si="0"/>
+        <v>1112.3333333333333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>55</v>
       </c>
@@ -1010,8 +1055,12 @@
       <c r="L16" s="1">
         <v>110.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="8">
+        <f t="shared" si="0"/>
+        <v>1184.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>60</v>
       </c>
@@ -1048,8 +1097,12 @@
       <c r="L17" s="1">
         <v>114.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="8">
+        <f t="shared" si="0"/>
+        <v>1256.3666666666666</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>65</v>
       </c>
@@ -1086,8 +1139,12 @@
       <c r="L18" s="1">
         <v>123.8</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="8">
+        <f t="shared" si="0"/>
+        <v>1328.3333333333333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>70</v>
       </c>
@@ -1124,8 +1181,12 @@
       <c r="L19" s="1">
         <v>130.69999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" s="8">
+        <f t="shared" si="0"/>
+        <v>1400.3666666666668</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>75</v>
       </c>
@@ -1162,8 +1223,12 @@
       <c r="L20" s="1">
         <v>138</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="8">
+        <f t="shared" si="0"/>
+        <v>1472.3333333333333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>80</v>
       </c>
@@ -1200,8 +1265,12 @@
       <c r="L21" s="1">
         <v>146.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" s="8">
+        <f t="shared" si="0"/>
+        <v>1543.8000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>85</v>
       </c>
@@ -1238,8 +1307,12 @@
       <c r="L22" s="1">
         <v>155.6</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" s="8">
+        <f t="shared" si="0"/>
+        <v>1615.2333333333333</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>90</v>
       </c>
@@ -1276,8 +1349,12 @@
       <c r="L23" s="1">
         <v>167</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" s="8">
+        <f t="shared" si="0"/>
+        <v>1690.2333333333333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>91.2</v>
       </c>
@@ -1314,8 +1391,12 @@
       <c r="L24" s="1">
         <v>183</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24" s="8">
+        <f t="shared" si="0"/>
+        <v>1765.2333333333333</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>95</v>
       </c>
@@ -1352,8 +1433,12 @@
       <c r="L25" s="1">
         <v>191.2</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" s="8">
+        <f t="shared" si="0"/>
+        <v>1840.2333333333333</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>99.9</v>
       </c>
@@ -1389,6 +1474,10 @@
       </c>
       <c r="L26" s="1">
         <v>209</v>
+      </c>
+      <c r="M26" s="8">
+        <f t="shared" si="0"/>
+        <v>1915.2333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>